<commit_message>
Update demo game setting.
</commit_message>
<xml_diff>
--- a/biosim_server_beta/example_game_bee.xlsx
+++ b/biosim_server_beta/example_game_bee.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shenshenmac/codes/biosim_servers/biosim_server_beta/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="0" windowWidth="25600" windowHeight="15700" tabRatio="500"/>
+    <workbookView xWindow="1440" yWindow="460" windowWidth="25600" windowHeight="15700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="biosim-setup" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'biosim-setup'!$A$4:$W$12</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
     <t>Game Holder Name</t>
   </si>
@@ -183,9 +188,6 @@
     <t>flower-2</t>
   </si>
   <si>
-    <t>flower-6</t>
-  </si>
-  <si>
     <t>flower-5</t>
   </si>
   <si>
@@ -241,6 +243,9 @@
   <si>
     <t>sam,shenshen</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flower-7</t>
   </si>
 </sst>
 </file>
@@ -400,26 +405,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="39">
-    <cellStyle name="普通" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -439,6 +425,25 @@
     <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="86">
     <dxf>
@@ -1644,11 +1649,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" customWidth="1"/>
@@ -1669,7 +1674,7 @@
     <col min="23" max="23" width="18.1640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="56" customHeight="1">
+    <row r="1" spans="1:23" ht="56" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1686,7 +1691,7 @@
         <v>33</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>28</v>
@@ -1711,9 +1716,9 @@
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
     </row>
-    <row r="2" spans="1:23" ht="15" customHeight="1">
+    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="7">
         <v>14</v>
@@ -1722,7 +1727,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="7">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="E2" s="7">
         <v>3</v>
@@ -1753,7 +1758,7 @@
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="1:23" ht="61" customHeight="1">
+    <row r="3" spans="1:23" ht="61" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1773,7 +1778,7 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" ht="55" customHeight="1">
+    <row r="4" spans="1:23" s="1" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -1793,7 +1798,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>9</v>
@@ -1802,7 +1807,7 @@
         <v>10</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>23</v>
@@ -1811,13 +1816,13 @@
         <v>25</v>
       </c>
       <c r="M4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>12</v>
@@ -1826,7 +1831,7 @@
         <v>11</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>14</v>
@@ -1844,12 +1849,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15" customHeight="1">
+    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="5">
         <v>3</v>
@@ -1858,7 +1863,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F5" s="5">
         <v>3</v>
@@ -1874,7 +1879,7 @@
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -1891,13 +1896,13 @@
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
       <c r="V5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="W5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="W5" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1">
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
@@ -1911,10 +1916,10 @@
         <v>13</v>
       </c>
       <c r="E6" s="5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F6" s="5">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
@@ -1945,7 +1950,7 @@
       <c r="V6" s="12"/>
       <c r="W6" s="9"/>
     </row>
-    <row r="7" spans="1:23" ht="15" customHeight="1">
+    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="5"/>
@@ -1981,9 +1986,9 @@
       <c r="V7" s="12"/>
       <c r="W7" s="9"/>
     </row>
-    <row r="8" spans="1:23" ht="15" customHeight="1">
+    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>22</v>
@@ -1992,16 +1997,16 @@
         <v>1</v>
       </c>
       <c r="D8" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E8" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="5">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G8" s="5">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -2013,7 +2018,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>18</v>
@@ -2031,7 +2036,7 @@
       <c r="V8" s="12"/>
       <c r="W8" s="9"/>
     </row>
-    <row r="9" spans="1:23" ht="15" customHeight="1">
+    <row r="9" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
@@ -2042,16 +2047,16 @@
         <v>1</v>
       </c>
       <c r="D9" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E9" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F9" s="5">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G9" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -2063,7 +2068,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="P9" s="5" t="s">
         <v>18</v>
@@ -2081,16 +2086,12 @@
       <c r="V9" s="12"/>
       <c r="W9" s="9"/>
     </row>
-    <row r="10" spans="1:23" ht="15" customHeight="1">
+    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="5">
         <v>5</v>
       </c>
@@ -2113,7 +2114,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P10" s="5" t="s">
         <v>18</v>
@@ -2131,7 +2132,7 @@
       <c r="V10" s="12"/>
       <c r="W10" s="9"/>
     </row>
-    <row r="11" spans="1:23" ht="15" customHeight="1">
+    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2172,9 +2173,9 @@
       <c r="V11" s="12"/>
       <c r="W11" s="9"/>
     </row>
-    <row r="12" spans="1:23" ht="15" customHeight="1">
+    <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>15</v>
@@ -2186,10 +2187,10 @@
         <v>2</v>
       </c>
       <c r="E12" s="5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F12" s="5">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="G12" s="5">
         <v>0</v>
@@ -2220,12 +2221,12 @@
       <c r="V12" s="12"/>
       <c r="W12" s="9"/>
     </row>
-    <row r="13" spans="1:23" ht="15" customHeight="1">
+    <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="5">
         <v>3</v>
@@ -2234,7 +2235,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F13" s="5">
         <v>3</v>
@@ -2250,7 +2251,7 @@
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -2270,7 +2271,7 @@
       <c r="V13" s="12"/>
       <c r="W13" s="9"/>
     </row>
-    <row r="14" spans="1:23" ht="15" customHeight="1">
+    <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
@@ -2295,7 +2296,7 @@
       <c r="V14" s="12"/>
       <c r="W14" s="9"/>
     </row>
-    <row r="15" spans="1:23" ht="15" customHeight="1">
+    <row r="15" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2323,7 +2324,7 @@
       <c r="V15" s="12"/>
       <c r="W15" s="9"/>
     </row>
-    <row r="16" spans="1:23" ht="15" customHeight="1">
+    <row r="16" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2351,7 +2352,7 @@
       <c r="V16" s="12"/>
       <c r="W16" s="9"/>
     </row>
-    <row r="17" spans="1:23" ht="15" customHeight="1">
+    <row r="17" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2379,7 +2380,7 @@
       <c r="V17" s="12"/>
       <c r="W17" s="9"/>
     </row>
-    <row r="18" spans="1:23" ht="15" customHeight="1">
+    <row r="18" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2407,7 +2408,7 @@
       <c r="V18" s="12"/>
       <c r="W18" s="9"/>
     </row>
-    <row r="19" spans="1:23" ht="15" customHeight="1">
+    <row r="19" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2435,7 +2436,7 @@
       <c r="V19" s="12"/>
       <c r="W19" s="9"/>
     </row>
-    <row r="20" spans="1:23" ht="15" customHeight="1">
+    <row r="20" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2463,7 +2464,7 @@
       <c r="V20" s="12"/>
       <c r="W20" s="9"/>
     </row>
-    <row r="21" spans="1:23" ht="15" customHeight="1">
+    <row r="21" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2491,7 +2492,7 @@
       <c r="V21" s="12"/>
       <c r="W21" s="9"/>
     </row>
-    <row r="22" spans="1:23" ht="15" customHeight="1">
+    <row r="22" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2519,7 +2520,7 @@
       <c r="V22" s="12"/>
       <c r="W22" s="9"/>
     </row>
-    <row r="23" spans="1:23" ht="15" customHeight="1">
+    <row r="23" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2547,7 +2548,7 @@
       <c r="V23" s="12"/>
       <c r="W23" s="9"/>
     </row>
-    <row r="24" spans="1:23" ht="15" customHeight="1">
+    <row r="24" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2575,7 +2576,7 @@
       <c r="V24" s="12"/>
       <c r="W24" s="9"/>
     </row>
-    <row r="25" spans="1:23" ht="15" customHeight="1">
+    <row r="25" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2603,7 +2604,7 @@
       <c r="V25" s="12"/>
       <c r="W25" s="9"/>
     </row>
-    <row r="26" spans="1:23" ht="15" customHeight="1">
+    <row r="26" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2631,7 +2632,7 @@
       <c r="V26" s="12"/>
       <c r="W26" s="9"/>
     </row>
-    <row r="27" spans="1:23" ht="15" customHeight="1">
+    <row r="27" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2659,7 +2660,7 @@
       <c r="V27" s="12"/>
       <c r="W27" s="9"/>
     </row>
-    <row r="28" spans="1:23" ht="15" customHeight="1">
+    <row r="28" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2687,7 +2688,7 @@
       <c r="V28" s="12"/>
       <c r="W28" s="9"/>
     </row>
-    <row r="29" spans="1:23" ht="15" customHeight="1">
+    <row r="29" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2715,7 +2716,7 @@
       <c r="V29" s="12"/>
       <c r="W29" s="9"/>
     </row>
-    <row r="30" spans="1:23" ht="15" customHeight="1">
+    <row r="30" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2743,7 +2744,7 @@
       <c r="V30" s="12"/>
       <c r="W30" s="9"/>
     </row>
-    <row r="31" spans="1:23" ht="15" customHeight="1">
+    <row r="31" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2771,7 +2772,7 @@
       <c r="V31" s="12"/>
       <c r="W31" s="9"/>
     </row>
-    <row r="32" spans="1:23" ht="15" customHeight="1">
+    <row r="32" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2799,7 +2800,7 @@
       <c r="V32" s="12"/>
       <c r="W32" s="9"/>
     </row>
-    <row r="33" spans="1:23" ht="15" customHeight="1">
+    <row r="33" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2827,7 +2828,7 @@
       <c r="V33" s="12"/>
       <c r="W33" s="9"/>
     </row>
-    <row r="34" spans="1:23" ht="15" customHeight="1">
+    <row r="34" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2855,7 +2856,7 @@
       <c r="V34" s="12"/>
       <c r="W34" s="9"/>
     </row>
-    <row r="35" spans="1:23" ht="15" customHeight="1">
+    <row r="35" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2883,7 +2884,7 @@
       <c r="V35" s="12"/>
       <c r="W35" s="9"/>
     </row>
-    <row r="36" spans="1:23" ht="15" customHeight="1">
+    <row r="36" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2911,7 +2912,7 @@
       <c r="V36" s="12"/>
       <c r="W36" s="9"/>
     </row>
-    <row r="37" spans="1:23" ht="15" customHeight="1">
+    <row r="37" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -2939,7 +2940,7 @@
       <c r="V37" s="12"/>
       <c r="W37" s="9"/>
     </row>
-    <row r="38" spans="1:23" ht="15" customHeight="1">
+    <row r="38" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -2967,7 +2968,7 @@
       <c r="V38" s="12"/>
       <c r="W38" s="9"/>
     </row>
-    <row r="39" spans="1:23" ht="15" customHeight="1">
+    <row r="39" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2995,7 +2996,7 @@
       <c r="V39" s="12"/>
       <c r="W39" s="9"/>
     </row>
-    <row r="40" spans="1:23" ht="15" customHeight="1">
+    <row r="40" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -3456,10 +3457,5 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>